<commit_message>
Edit Readme.md - add detailed workflow of ipynb files and add blds-indicators.pynb
</commit_message>
<xml_diff>
--- a/indicators-data/population.xlsx
+++ b/indicators-data/population.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucnmuni-my.sharepoint.com/personal/436645_muni_cz/Documents/VŠ/PhD/Zahraniční stáž/Work/HeiGIT_notebooks/analysis/ai-assisted-osm-mapping-stats/indicators-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_F7E5F348454CBF5BF97E5152C12A46D867D6C741" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E20BF1CA-5A6A-4682-A217-61E1C09EC019}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F7E5F348454CBF5BF97E5152C12A46D867D6C741" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BD66CBD-B8BF-4449-9F24-84E19D6F5D02}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="Series - Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1'!$A$1:$I$267</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1621,9 +1624,6 @@
     <t>Morocco</t>
   </si>
   <si>
-    <t>Country Code</t>
-  </si>
-  <si>
     <t>LBN</t>
   </si>
   <si>
@@ -1718,6 +1718,9 @@
   </si>
   <si>
     <t>country</t>
+  </si>
+  <si>
+    <t>iso</t>
   </si>
 </sst>
 </file>
@@ -2065,11 +2068,14 @@
   <dimension ref="A1:I271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G275" sqref="G275"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2081,10 +2087,10 @@
         <v>445</v>
       </c>
       <c r="C1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>530</v>
       </c>
       <c r="E1">
         <v>2018</v>
@@ -2104,7 +2110,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>422</v>
@@ -2133,7 +2139,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>422</v>
@@ -2162,7 +2168,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>422</v>
@@ -2191,7 +2197,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>422</v>
@@ -2220,7 +2226,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>422</v>
@@ -2249,7 +2255,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>422</v>
@@ -2278,7 +2284,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>422</v>
@@ -2307,7 +2313,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>422</v>
@@ -2336,7 +2342,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>422</v>
@@ -2365,7 +2371,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>422</v>
@@ -2394,7 +2400,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>422</v>
@@ -2423,7 +2429,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>422</v>
@@ -2452,7 +2458,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>422</v>
@@ -2481,7 +2487,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>422</v>
@@ -2510,7 +2516,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>422</v>
@@ -2539,7 +2545,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>422</v>
@@ -2568,7 +2574,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>422</v>
@@ -2597,7 +2603,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>422</v>
@@ -2626,7 +2632,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>422</v>
@@ -2655,7 +2661,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>422</v>
@@ -2684,7 +2690,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>422</v>
@@ -2713,7 +2719,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>422</v>
@@ -2742,7 +2748,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>422</v>
@@ -2771,7 +2777,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>422</v>
@@ -2800,7 +2806,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>422</v>
@@ -2829,7 +2835,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>422</v>
@@ -2858,7 +2864,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>422</v>
@@ -2887,7 +2893,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>422</v>
@@ -2916,7 +2922,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>422</v>
@@ -2945,7 +2951,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>422</v>
@@ -2974,7 +2980,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>422</v>
@@ -3003,13 +3009,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>208</v>
@@ -3032,7 +3038,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>422</v>
@@ -3061,7 +3067,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>422</v>
@@ -3090,7 +3096,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>422</v>
@@ -3119,7 +3125,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>422</v>
@@ -3148,7 +3154,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>422</v>
@@ -3177,7 +3183,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>422</v>
@@ -3206,7 +3212,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>422</v>
@@ -3235,7 +3241,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>422</v>
@@ -3264,13 +3270,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C42" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>245</v>
@@ -3293,7 +3299,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>422</v>
@@ -3322,7 +3328,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>422</v>
@@ -3351,7 +3357,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>422</v>
@@ -3380,7 +3386,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>422</v>
@@ -3409,7 +3415,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>422</v>
@@ -3418,7 +3424,7 @@
         <v>156</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E47">
         <v>5441062</v>
@@ -3438,7 +3444,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>422</v>
@@ -3467,7 +3473,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>422</v>
@@ -3496,13 +3502,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>544</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C50" t="s">
         <v>545</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C50" t="s">
-        <v>546</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>5</v>
@@ -3525,7 +3531,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>422</v>
@@ -3554,7 +3560,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>422</v>
@@ -3583,7 +3589,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>422</v>
@@ -3612,7 +3618,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>422</v>
@@ -3641,7 +3647,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>422</v>
@@ -3670,7 +3676,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>422</v>
@@ -3699,7 +3705,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>422</v>
@@ -3708,7 +3714,7 @@
         <v>117</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E57">
         <v>70823</v>
@@ -3728,7 +3734,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>422</v>
@@ -3757,7 +3763,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>422</v>
@@ -3786,7 +3792,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>422</v>
@@ -3815,7 +3821,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>422</v>
@@ -3844,7 +3850,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>422</v>
@@ -3873,7 +3879,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>422</v>
@@ -3902,7 +3908,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>422</v>
@@ -3931,7 +3937,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>422</v>
@@ -3960,7 +3966,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>422</v>
@@ -3989,7 +3995,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>422</v>
@@ -4018,7 +4024,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>422</v>
@@ -4047,7 +4053,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>422</v>
@@ -4076,7 +4082,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>422</v>
@@ -4105,7 +4111,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>422</v>
@@ -4134,7 +4140,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>422</v>
@@ -4163,7 +4169,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>422</v>
@@ -4172,7 +4178,7 @@
         <v>293</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E73">
         <v>2444916</v>
@@ -4192,7 +4198,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>422</v>
@@ -4221,7 +4227,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>422</v>
@@ -4250,7 +4256,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>422</v>
@@ -4279,7 +4285,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>422</v>
@@ -4308,7 +4314,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>422</v>
@@ -4337,7 +4343,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>422</v>
@@ -4366,7 +4372,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>422</v>
@@ -4395,7 +4401,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>422</v>
@@ -4424,7 +4430,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>422</v>
@@ -4453,7 +4459,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>422</v>
@@ -4482,7 +4488,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>422</v>
@@ -4511,7 +4517,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>422</v>
@@ -4540,7 +4546,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>422</v>
@@ -4569,7 +4575,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>422</v>
@@ -4598,7 +4604,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>422</v>
@@ -4627,7 +4633,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>422</v>
@@ -4656,7 +4662,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>422</v>
@@ -4685,7 +4691,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>422</v>
@@ -4714,7 +4720,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>422</v>
@@ -4743,7 +4749,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>422</v>
@@ -4772,7 +4778,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>422</v>
@@ -4801,7 +4807,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>422</v>
@@ -4830,7 +4836,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>422</v>
@@ -4859,7 +4865,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>422</v>
@@ -4888,7 +4894,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>422</v>
@@ -4917,7 +4923,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>422</v>
@@ -4946,7 +4952,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>422</v>
@@ -4975,7 +4981,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>422</v>
@@ -5004,7 +5010,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>422</v>
@@ -5033,7 +5039,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>422</v>
@@ -5062,7 +5068,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>422</v>
@@ -5091,7 +5097,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>422</v>
@@ -5120,7 +5126,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>422</v>
@@ -5149,7 +5155,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>422</v>
@@ -5178,7 +5184,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>422</v>
@@ -5207,7 +5213,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>422</v>
@@ -5236,7 +5242,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>422</v>
@@ -5265,7 +5271,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>422</v>
@@ -5294,7 +5300,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>422</v>
@@ -5303,7 +5309,7 @@
         <v>33</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E112">
         <v>5950839</v>
@@ -5323,7 +5329,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>422</v>
@@ -5352,7 +5358,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>422</v>
@@ -5381,7 +5387,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>422</v>
@@ -5410,7 +5416,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>422</v>
@@ -5439,7 +5445,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>422</v>
@@ -5468,7 +5474,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>422</v>
@@ -5497,7 +5503,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>422</v>
@@ -5526,7 +5532,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>422</v>
@@ -5555,7 +5561,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>422</v>
@@ -5584,7 +5590,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>422</v>
@@ -5593,7 +5599,7 @@
         <v>268</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E122">
         <v>32399271</v>
@@ -5613,7 +5619,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>422</v>
@@ -5642,7 +5648,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>422</v>
@@ -5671,7 +5677,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>422</v>
@@ -5700,7 +5706,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>422</v>
@@ -5729,7 +5735,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>422</v>
@@ -5758,7 +5764,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>422</v>
@@ -5787,7 +5793,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>422</v>
@@ -5816,7 +5822,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>422</v>
@@ -5825,7 +5831,7 @@
         <v>278</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E130">
         <v>110929</v>
@@ -5845,7 +5851,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>422</v>
@@ -5854,7 +5860,7 @@
         <v>175</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E131">
         <v>2707203</v>
@@ -5874,7 +5880,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>422</v>
@@ -5903,7 +5909,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>422</v>
@@ -5932,7 +5938,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>422</v>
@@ -5961,7 +5967,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>422</v>
@@ -5990,7 +5996,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>422</v>
@@ -6019,7 +6025,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>422</v>
@@ -6048,7 +6054,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>422</v>
@@ -6077,7 +6083,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>422</v>
@@ -6106,7 +6112,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>422</v>
@@ -6135,7 +6141,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>422</v>
@@ -6164,7 +6170,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>422</v>
@@ -6193,7 +6199,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>422</v>
@@ -6222,7 +6228,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>422</v>
@@ -6251,7 +6257,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>422</v>
@@ -6280,7 +6286,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>422</v>
@@ -6309,7 +6315,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>422</v>
@@ -6338,7 +6344,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>422</v>
@@ -6367,7 +6373,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>422</v>
@@ -6396,7 +6402,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>422</v>
@@ -6425,13 +6431,13 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C151" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>388</v>
@@ -6454,7 +6460,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>422</v>
@@ -6483,7 +6489,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>422</v>
@@ -6512,7 +6518,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>422</v>
@@ -6541,7 +6547,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>422</v>
@@ -6570,7 +6576,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>422</v>
@@ -6599,7 +6605,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>422</v>
@@ -6628,7 +6634,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>422</v>
@@ -6657,7 +6663,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>422</v>
@@ -6686,7 +6692,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>422</v>
@@ -6715,7 +6721,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>422</v>
@@ -6744,7 +6750,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>422</v>
@@ -6773,7 +6779,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>422</v>
@@ -6802,7 +6808,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>422</v>
@@ -6831,7 +6837,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>422</v>
@@ -6860,7 +6866,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>422</v>
@@ -6889,7 +6895,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>422</v>
@@ -6918,7 +6924,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>422</v>
@@ -6947,7 +6953,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>422</v>
@@ -6976,13 +6982,13 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C170" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>197</v>
@@ -7005,7 +7011,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>422</v>
@@ -7034,7 +7040,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>422</v>
@@ -7063,7 +7069,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>422</v>
@@ -7092,7 +7098,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>422</v>
@@ -7121,7 +7127,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>422</v>
@@ -7150,7 +7156,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>422</v>
@@ -7179,7 +7185,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>422</v>
@@ -7208,7 +7214,7 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>422</v>
@@ -7237,7 +7243,7 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>422</v>
@@ -7266,7 +7272,7 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>422</v>
@@ -7295,7 +7301,7 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>422</v>
@@ -7324,7 +7330,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>422</v>
@@ -7353,7 +7359,7 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>422</v>
@@ -7362,7 +7368,7 @@
         <v>443</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E183">
         <v>47761</v>
@@ -7382,7 +7388,7 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>422</v>
@@ -7411,13 +7417,13 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C185" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>495</v>
@@ -7440,7 +7446,7 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>422</v>
@@ -7469,7 +7475,7 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>422</v>
@@ -7498,7 +7504,7 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>422</v>
@@ -7527,7 +7533,7 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>422</v>
@@ -7556,7 +7562,7 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>422</v>
@@ -7585,7 +7591,7 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>422</v>
@@ -7614,7 +7620,7 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>422</v>
@@ -7643,7 +7649,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>422</v>
@@ -7672,13 +7678,13 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C194" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>357</v>
@@ -7701,7 +7707,7 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>422</v>
@@ -7730,7 +7736,7 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>422</v>
@@ -7759,7 +7765,7 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>422</v>
@@ -7788,7 +7794,7 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>422</v>
@@ -7817,13 +7823,13 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C199" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>98</v>
@@ -7846,7 +7852,7 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>422</v>
@@ -7875,7 +7881,7 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>422</v>
@@ -7904,13 +7910,13 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C202" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>528</v>
@@ -7933,7 +7939,7 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>422</v>
@@ -7942,7 +7948,7 @@
         <v>116</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E203">
         <v>10865</v>
@@ -7962,7 +7968,7 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>422</v>
@@ -7991,7 +7997,7 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>422</v>
@@ -8020,7 +8026,7 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>422</v>
@@ -8049,7 +8055,7 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>422</v>
@@ -8078,7 +8084,7 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>422</v>
@@ -8107,7 +8113,7 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>422</v>
@@ -8136,7 +8142,7 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>422</v>
@@ -8165,7 +8171,7 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>422</v>
@@ -8194,7 +8200,7 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>422</v>
@@ -8223,7 +8229,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>422</v>
@@ -8232,7 +8238,7 @@
         <v>281</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E213">
         <v>94914330</v>
@@ -8252,7 +8258,7 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>422</v>
@@ -8281,7 +8287,7 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>422</v>
@@ -8310,7 +8316,7 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>422</v>
@@ -8339,7 +8345,7 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>422</v>
@@ -8368,7 +8374,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>422</v>
@@ -8397,7 +8403,7 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>422</v>
@@ -8426,7 +8432,7 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>422</v>
@@ -8455,7 +8461,7 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>422</v>
@@ -8484,7 +8490,7 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>422</v>
@@ -8513,7 +8519,7 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>422</v>
@@ -8542,7 +8548,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>422</v>
@@ -8551,7 +8557,7 @@
         <v>353</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E224">
         <v>3294298709</v>
@@ -8571,7 +8577,7 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>422</v>
@@ -8600,7 +8606,7 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>422</v>
@@ -8629,7 +8635,7 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>422</v>
@@ -8658,7 +8664,7 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>422</v>
@@ -8667,7 +8673,7 @@
         <v>383</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E228">
         <v>342065158</v>
@@ -8687,7 +8693,7 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>422</v>
@@ -8716,7 +8722,7 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>422</v>
@@ -8725,7 +8731,7 @@
         <v>409</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E230">
         <v>398076771</v>
@@ -8745,7 +8751,7 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>422</v>
@@ -8774,7 +8780,7 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>422</v>
@@ -8803,7 +8809,7 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>422</v>
@@ -8832,7 +8838,7 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>422</v>
@@ -8861,7 +8867,7 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>422</v>
@@ -8890,7 +8896,7 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>422</v>
@@ -8899,7 +8905,7 @@
         <v>444</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E236">
         <v>4795957754</v>
@@ -8919,7 +8925,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>422</v>
@@ -8948,7 +8954,7 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>422</v>
@@ -8977,7 +8983,7 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>422</v>
@@ -9006,7 +9012,7 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>422</v>
@@ -9035,7 +9041,7 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>422</v>
@@ -9064,7 +9070,7 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>422</v>
@@ -9093,7 +9099,7 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>422</v>
@@ -9122,7 +9128,7 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>422</v>
@@ -9151,7 +9157,7 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>422</v>
@@ -9180,7 +9186,7 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>422</v>
@@ -9209,7 +9215,7 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>422</v>
@@ -9238,7 +9244,7 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>422</v>
@@ -9267,7 +9273,7 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>422</v>
@@ -9296,7 +9302,7 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>422</v>
@@ -9325,7 +9331,7 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>422</v>
@@ -9354,7 +9360,7 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>422</v>
@@ -9383,7 +9389,7 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>422</v>
@@ -9412,7 +9418,7 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>422</v>
@@ -9441,7 +9447,7 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>422</v>
@@ -9470,7 +9476,7 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>422</v>
@@ -9499,7 +9505,7 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>422</v>
@@ -9528,7 +9534,7 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>422</v>
@@ -9557,7 +9563,7 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>422</v>
@@ -9586,7 +9592,7 @@
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>422</v>
@@ -9615,7 +9621,7 @@
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>422</v>
@@ -9644,7 +9650,7 @@
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>422</v>
@@ -9673,16 +9679,16 @@
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C263" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E263">
         <v>1092403699</v>
@@ -9702,7 +9708,7 @@
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>422</v>
@@ -9731,7 +9737,7 @@
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>422</v>
@@ -9760,7 +9766,7 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>422</v>
@@ -9789,7 +9795,7 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>422</v>
@@ -9798,7 +9804,7 @@
         <v>149</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E267">
         <v>7661776338</v>
@@ -9833,6 +9839,7 @@
       <c r="D271" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I267" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9872,13 +9879,13 @@
         <v>147</v>
       </c>
       <c r="H1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I1" t="s">
         <v>271</v>
       </c>
       <c r="J1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K1" t="s">
         <v>330</v>
@@ -9898,16 +9905,16 @@
         <v>519</v>
       </c>
       <c r="C2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E2" t="s">
         <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G2" t="s">
         <v>180</v>

</xml_diff>